<commit_message>
DP-2544-add different dataset to second tab and rename tabs
</commit_message>
<xml_diff>
--- a/example/data/input/data-with-multiple-tabs.xlsx
+++ b/example/data/input/data-with-multiple-tabs.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DataPipline\Cloned\RealClone\DataPipeline-Examples\example\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4281EA-975F-42FF-964E-580F6D215CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2BD667-A3DA-449A-B825-90B48587F2A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Agents Information" sheetId="1" r:id="rId1"/>
+    <sheet name="Countries" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
   <si>
     <t>event_type</t>
   </si>
@@ -69,6 +69,33 @@
   </si>
   <si>
     <t>WARM_TRANSFER</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Addres</t>
+  </si>
+  <si>
+    <t>101 Independecne Avenue</t>
+  </si>
+  <si>
+    <t>15205 North Kierland</t>
+  </si>
+  <si>
+    <t>2796 Reserve St</t>
+  </si>
+  <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>ul. Gdańca Pawła 36</t>
   </si>
 </sst>
 </file>
@@ -426,11 +453,13 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
     <col min="5" max="5" width="20.7109375" customWidth="1"/>
     <col min="6" max="6" width="17.140625" customWidth="1"/>
   </cols>
@@ -625,198 +654,121 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A8FF550-9AA4-4F7B-803E-9437ED50CC05}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G14" sqref="G13:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="3">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3">
-        <v>340</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1">
-        <v>42447.882957384259</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="3">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3">
-        <v>340</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1">
-        <v>42447.882957384259</v>
-      </c>
-      <c r="F3" s="1">
-        <v>42447.882980983799</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3">
-        <v>6</v>
-      </c>
-      <c r="C4" s="3">
-        <v>315</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="1">
-        <v>42447.883004282405</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="3">
-        <v>6</v>
-      </c>
-      <c r="C5" s="3">
-        <v>315</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="1">
-        <v>42447.883004282405</v>
-      </c>
-      <c r="F5" s="1">
-        <v>42447.883027546297</v>
-      </c>
-      <c r="G5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="3">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3">
-        <v>334</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="1">
-        <v>42447.883050787037</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="3">
-        <v>7</v>
-      </c>
-      <c r="C7" s="3">
-        <v>334</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="1">
-        <v>42447.883050787037</v>
-      </c>
-      <c r="F7" s="1">
-        <v>42447.883074050929</v>
-      </c>
-      <c r="G7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3">
-        <v>8</v>
-      </c>
-      <c r="C8" s="3">
-        <v>323</v>
-      </c>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="1">
-        <v>42447.883097291669</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="3">
-        <v>8</v>
-      </c>
-      <c r="C9" s="3">
-        <v>323</v>
-      </c>
-      <c r="D9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="1">
-        <v>42447.883097291669</v>
-      </c>
-      <c r="F9" s="1">
-        <v>42447.88312053241</v>
-      </c>
-      <c r="G9" t="s">
-        <v>15</v>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DP-2544-change mispelled address name
</commit_message>
<xml_diff>
--- a/example/data/input/data-with-multiple-tabs.xlsx
+++ b/example/data/input/data-with-multiple-tabs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DataPipline\Cloned\RealClone\DataPipeline-Examples\example\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2BD667-A3DA-449A-B825-90B48587F2A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1994B94D-947D-4355-B45F-02B7C311EF23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,9 +80,6 @@
     <t>Canada</t>
   </si>
   <si>
-    <t>Addres</t>
-  </si>
-  <si>
     <t>101 Independecne Avenue</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>ul. Gdańca Pawła 36</t>
+  </si>
+  <si>
+    <t>address</t>
   </si>
 </sst>
 </file>
@@ -657,7 +657,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G13:G14"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,7 +676,7 @@
         <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -687,7 +687,7 @@
         <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -698,7 +698,7 @@
         <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -709,7 +709,7 @@
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -720,7 +720,7 @@
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -731,7 +731,7 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -742,7 +742,7 @@
         <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -750,10 +750,10 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
         <v>23</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -761,10 +761,10 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
         <v>23</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>